<commit_message>
added support for running mfd (medial axis) from python
</commit_message>
<xml_diff>
--- a/statistics/statistics_70_3_200_1.xlsx
+++ b/statistics/statistics_70_3_200_1.xlsx
@@ -487,10 +487,10 @@
         <v>17.94827906481845</v>
       </c>
       <c r="G2">
-        <v>74.13038727351888</v>
+        <v>75.17253906259769</v>
       </c>
       <c r="H2">
-        <v>4.130222569295041</v>
+        <v>4.188286731620309</v>
       </c>
       <c r="I2">
         <v>70</v>
@@ -528,10 +528,10 @@
         <v>20.77616515624208</v>
       </c>
       <c r="G3">
-        <v>50.17672378122897</v>
+        <v>41.45877320543772</v>
       </c>
       <c r="H3">
-        <v>2.415109978376047</v>
+        <v>1.995496902034478</v>
       </c>
       <c r="I3">
         <v>70</v>
@@ -569,10 +569,10 @@
         <v>22.2208554891313</v>
       </c>
       <c r="G4">
-        <v>33.19209777852731</v>
+        <v>32.82951004874731</v>
       </c>
       <c r="H4">
-        <v>1.493736269279204</v>
+        <v>1.477418817867068</v>
       </c>
       <c r="I4">
         <v>70</v>
@@ -610,10 +610,10 @@
         <v>21.83031551491332</v>
       </c>
       <c r="G5">
-        <v>42.92899481035813</v>
+        <v>38.99693567293362</v>
       </c>
       <c r="H5">
-        <v>1.966485311723109</v>
+        <v>1.786366103883976</v>
       </c>
       <c r="I5">
         <v>70</v>
@@ -651,10 +651,10 @@
         <v>15.54900450208879</v>
       </c>
       <c r="G6">
-        <v>45.57913575763984</v>
+        <v>42.62121031591623</v>
       </c>
       <c r="H6">
-        <v>2.931321793077938</v>
+        <v>2.741089328914315</v>
       </c>
       <c r="I6">
         <v>70</v>
@@ -692,10 +692,10 @@
         <v>112.6966620646871</v>
       </c>
       <c r="G7">
-        <v>88.52894011154999</v>
+        <v>90.17548792134531</v>
       </c>
       <c r="H7">
-        <v>0.785550685261068</v>
+        <v>0.8001611251767615</v>
       </c>
       <c r="I7">
         <v>70</v>
@@ -733,10 +733,10 @@
         <v>10.42763777637533</v>
       </c>
       <c r="G8">
-        <v>43.19834984425776</v>
+        <v>45.79194179155397</v>
       </c>
       <c r="H8">
-        <v>4.142678406237623</v>
+        <v>4.391401271657076</v>
       </c>
       <c r="I8">
         <v>70</v>
@@ -774,10 +774,10 @@
         <v>9.598159591780577</v>
       </c>
       <c r="G9">
-        <v>37.71785038847172</v>
+        <v>42.4338049218881</v>
       </c>
       <c r="H9">
-        <v>3.929696107655009</v>
+        <v>4.421035565841859</v>
       </c>
       <c r="I9">
         <v>70</v>
@@ -815,10 +815,10 @@
         <v>11.20370667039757</v>
       </c>
       <c r="G10">
-        <v>32.94529266697958</v>
+        <v>30.85314796492898</v>
       </c>
       <c r="H10">
-        <v>2.940570798236589</v>
+        <v>2.753833965186642</v>
       </c>
       <c r="I10">
         <v>70</v>
@@ -856,10 +856,10 @@
         <v>16.45652920812255</v>
       </c>
       <c r="G11">
-        <v>50.11049156865052</v>
+        <v>50.17943710733019</v>
       </c>
       <c r="H11">
-        <v>3.045021883710277</v>
+        <v>3.049211438980877</v>
       </c>
       <c r="I11">
         <v>70</v>
@@ -897,10 +897,10 @@
         <v>12.77569742324418</v>
       </c>
       <c r="G12">
-        <v>43.73606092817804</v>
+        <v>42.92282107595251</v>
       </c>
       <c r="H12">
-        <v>3.423379521231021</v>
+        <v>3.359724299501527</v>
       </c>
       <c r="I12">
         <v>70</v>
@@ -938,10 +938,10 @@
         <v>8.049231226310987</v>
       </c>
       <c r="G13">
-        <v>37.27480990676797</v>
+        <v>33.68210803386253</v>
       </c>
       <c r="H13">
-        <v>4.630853414289509</v>
+        <v>4.184512419492172</v>
       </c>
       <c r="I13">
         <v>70</v>

</xml_diff>